<commit_message>
complete keyword with reports
</commit_message>
<xml_diff>
--- a/resources/testcases.xlsx
+++ b/resources/testcases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -203,9 +203,6 @@
     <t>lst_Branch</t>
   </si>
   <si>
-    <t>Lingampalli</t>
-  </si>
-  <si>
     <t>BtnSubmit</t>
   </si>
   <si>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Btn_Reset</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +620,7 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,12 +628,12 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -661,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1027,7 @@
         <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,7 +1041,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -1074,7 +1077,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -1091,7 +1094,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
@@ -1131,10 +1134,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" t="s">
-        <v>65</v>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>